<commit_message>
atualizado dicionário de dados com modelo lógico
</commit_message>
<xml_diff>
--- a/Banco de Dados/Dicionario de dados.xlsx
+++ b/Banco de Dados/Dicionario de dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\princesa\Documents\Bandtec\GIT-Bandtec\grupo9-ads\Banco de Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teodoro\Desktop\grupo9-ads\Banco de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEF0CDC-81AD-455F-A443-1D8EF7CE5489}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8A22A6-4A21-447A-B736-D55EE24A1E63}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{8216B3B1-9DBC-447D-A8C2-D089C8F8847B}"/>
+    <workbookView xWindow="525" yWindow="30" windowWidth="15375" windowHeight="7875" xr2:uid="{8216B3B1-9DBC-447D-A8C2-D089C8F8847B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="63">
   <si>
     <t>dominio</t>
   </si>
@@ -211,22 +211,23 @@
   </si>
   <si>
     <t>xx.xxx.xxx/xxxx-xx</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>apelido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nome da geladeira para interpretar tipo de medicamento </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -238,6 +239,23 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -266,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -283,16 +301,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -301,12 +322,6 @@
   </cellStyles>
   <dxfs count="36">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -340,7 +355,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -373,52 +388,58 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -440,64 +461,64 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C4D8B25-9FD8-485D-87A6-95211DD7C718}" name="Tabela3" displayName="Tabela3" ref="A2:G8" totalsRowShown="0" headerRowDxfId="27" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C4D8B25-9FD8-485D-87A6-95211DD7C718}" name="Tabela3" displayName="Tabela3" ref="A2:G8" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A2:G8" xr:uid="{5863D25D-0C8A-4ADE-BFAD-B8DBBBE361D8}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3B4A6A92-2C9F-4F6C-9A7A-C8557925F3CE}" name="nome" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{8364ECD7-B0A8-4E4A-A427-B9C8E2CE5BB4}" name="descrição" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{21EA17A4-77DA-48B8-8C3F-8C8645064AB3}" name="tipo" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{5B6CBB9A-BD96-4AA9-A9B7-17FFF7F08617}" name="tamanho" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{B21A5A70-D7BA-491F-80BD-C374099C170E}" name="dominio" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{F674E7B7-78CB-4310-9AB5-12F91D3B5252}" name="formato" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{E2070883-DA67-4B1D-8608-995C122D861A}" name="restrições" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{3B4A6A92-2C9F-4F6C-9A7A-C8557925F3CE}" name="nome" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{8364ECD7-B0A8-4E4A-A427-B9C8E2CE5BB4}" name="descrição" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{21EA17A4-77DA-48B8-8C3F-8C8645064AB3}" name="tipo" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{5B6CBB9A-BD96-4AA9-A9B7-17FFF7F08617}" name="tamanho" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{B21A5A70-D7BA-491F-80BD-C374099C170E}" name="dominio" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{F674E7B7-78CB-4310-9AB5-12F91D3B5252}" name="formato" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{E2070883-DA67-4B1D-8608-995C122D861A}" name="restrições" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{046DC458-B0AF-4388-A866-63858DA16F8A}" name="Tabela4" displayName="Tabela4" ref="A11:G14" totalsRowShown="0" headerRowDxfId="18" dataDxfId="19">
-  <autoFilter ref="A11:G14" xr:uid="{CA082778-8308-4396-831D-1A415AA52195}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{046DC458-B0AF-4388-A866-63858DA16F8A}" name="Tabela4" displayName="Tabela4" ref="A11:G15" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="A11:G15" xr:uid="{CA082778-8308-4396-831D-1A415AA52195}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A576B442-BD0D-407D-8ADE-79B47E8C074D}" name="nome" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{D6087151-82BB-44C4-8D04-02FA93FDA407}" name="descrição" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{2661E471-8F90-4F72-A6CA-CBD7C1900159}" name="tipo" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{56A9376E-EFFB-4E88-8772-EA916EC5DEE9}" name="tamanho" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{538B5A28-264F-407C-8193-F12E93CCFCDF}" name="dominio" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{01F6DCA0-006C-4CE0-A7D4-C66F9FC50846}" name="formato" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{C7EB5DE2-2E0C-4790-B9D9-3D8892B1AC6E}" name="restrições" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{A576B442-BD0D-407D-8ADE-79B47E8C074D}" name="nome" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{D6087151-82BB-44C4-8D04-02FA93FDA407}" name="descrição" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{2661E471-8F90-4F72-A6CA-CBD7C1900159}" name="tipo" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{56A9376E-EFFB-4E88-8772-EA916EC5DEE9}" name="tamanho" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{538B5A28-264F-407C-8193-F12E93CCFCDF}" name="dominio" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{01F6DCA0-006C-4CE0-A7D4-C66F9FC50846}" name="formato" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{C7EB5DE2-2E0C-4790-B9D9-3D8892B1AC6E}" name="restrições" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{36A40C92-9B2C-47E1-A879-793EEEE4A3AE}" name="Tabela5" displayName="Tabela5" ref="A17:G23" totalsRowShown="0" headerRowDxfId="9" dataDxfId="10">
-  <autoFilter ref="A17:G23" xr:uid="{C20F07DA-1879-43D2-9775-26BB9DFEB828}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{36A40C92-9B2C-47E1-A879-793EEEE4A3AE}" name="Tabela5" displayName="Tabela5" ref="A18:G24" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A18:G24" xr:uid="{C20F07DA-1879-43D2-9775-26BB9DFEB828}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9023E542-B918-41FD-8985-4E4593BB3BD1}" name="nome" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{AA469F39-5722-4CCE-BF66-9891EA880B8E}" name="descrição" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{68875B3F-DFFA-4A8C-A5BE-1685E4BCB613}" name="tipo" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{61F54AE9-6BD2-466F-B77B-91666E1C4EA3}" name="tamanho" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{24D21FCC-16A6-4DE5-908C-10218E4C9129}" name="dominio" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{AB9B7C5C-7513-49AD-9605-5B464B09F87F}" name="formato" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{D2719BA9-DCAC-48BC-8195-33394EABF862}" name="restrições" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{9023E542-B918-41FD-8985-4E4593BB3BD1}" name="nome" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{AA469F39-5722-4CCE-BF66-9891EA880B8E}" name="descrição" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{68875B3F-DFFA-4A8C-A5BE-1685E4BCB613}" name="tipo" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{61F54AE9-6BD2-466F-B77B-91666E1C4EA3}" name="tamanho" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{24D21FCC-16A6-4DE5-908C-10218E4C9129}" name="dominio" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{AB9B7C5C-7513-49AD-9605-5B464B09F87F}" name="formato" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{D2719BA9-DCAC-48BC-8195-33394EABF862}" name="restrições" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C00E5A94-CBC5-4A3B-848A-BAA43508DCD7}" name="Tabela6" displayName="Tabela6" ref="A26:G31" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A26:G31" xr:uid="{17758034-83A2-4B20-889A-B72D23DF6F2F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C00E5A94-CBC5-4A3B-848A-BAA43508DCD7}" name="Tabela6" displayName="Tabela6" ref="A27:G32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A27:G32" xr:uid="{17758034-83A2-4B20-889A-B72D23DF6F2F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1384A437-A2FB-4CE9-BF0D-FA928434935D}" name="nome" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{9E89A8A5-89F8-4160-87DD-F5974F287CE6}" name="descrição" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{9E5BE7FF-71B6-4A6C-8C92-8BB29A438B24}" name="tipo" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{13C4CBB8-8325-4CDD-ADB8-3FB022F63D3F}" name="tamanho" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{24C262F8-9185-4600-BFD9-8DF2279812D0}" name="dominio" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{39B06816-A4CA-454F-8C08-8C273678A49B}" name="formato" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{B8B7D606-B2A7-4F69-A98A-3ED213FCA3DF}" name="restrições" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{1384A437-A2FB-4CE9-BF0D-FA928434935D}" name="nome" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{9E89A8A5-89F8-4160-87DD-F5974F287CE6}" name="descrição" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{9E5BE7FF-71B6-4A6C-8C92-8BB29A438B24}" name="tipo" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{13C4CBB8-8325-4CDD-ADB8-3FB022F63D3F}" name="tamanho" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{24C262F8-9185-4600-BFD9-8DF2279812D0}" name="dominio" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{39B06816-A4CA-454F-8C08-8C273678A49B}" name="formato" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{B8B7D606-B2A7-4F69-A98A-3ED213FCA3DF}" name="restrições" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -800,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70BB7CD9-6424-4AD5-94E5-5EE6407FF54C}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,15 +839,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -886,7 +907,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2">
         <v>4</v>
@@ -911,7 +932,7 @@
         <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2">
         <v>4</v>
@@ -1013,15 +1034,15 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
@@ -1073,35 +1094,31 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2">
+        <v>30</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2">
-        <v>11</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
@@ -1119,106 +1136,106 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <v>11</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="E19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <v>30</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="2">
-        <v>4</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>15</v>
@@ -1232,13 +1249,13 @@
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D21" s="2">
         <v>4</v>
@@ -1255,13 +1272,13 @@
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2">
         <v>4</v>
@@ -1278,13 +1295,13 @@
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D23" s="2">
         <v>4</v>
@@ -1299,79 +1316,79 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B27" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D28" s="1">
         <v>11</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="1">
-        <v>40</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>15</v>
@@ -1385,87 +1402,110 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D29" s="1">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>59</v>
+      <c r="F29" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D30" s="1">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>15</v>
+      <c r="F30" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="1">
+        <v>30</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="1">
         <v>10</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A26:G26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>